<commit_message>
Finish Get and Search
</commit_message>
<xml_diff>
--- a/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
+++ b/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
@@ -2266,7 +2266,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="AJ8" sqref="AJ7:AJ8"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="B7:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3061,17 +3061,17 @@
       <c r="A7" s="29" t="s">
         <v>538</v>
       </c>
-      <c r="B7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="10" t="b">
-        <v>0</v>
+      <c r="B7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="F7" s="6" t="b">
         <v>1</v>
@@ -3183,17 +3183,17 @@
     </row>
     <row r="8" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
-      <c r="B8" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10" t="b">
-        <v>0</v>
+      <c r="B8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="F8" s="6" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Fix BUG Process Service
</commit_message>
<xml_diff>
--- a/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
+++ b/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
@@ -2266,7 +2266,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3061,17 +3061,17 @@
       <c r="A7" s="29" t="s">
         <v>538</v>
       </c>
-      <c r="B7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6" t="b">
-        <v>1</v>
+      <c r="B7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="F7" s="6" t="b">
         <v>1</v>
@@ -3079,8 +3079,8 @@
       <c r="G7" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="10" t="b">
-        <v>0</v>
+      <c r="H7" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="I7" s="10" t="b">
         <v>0</v>
@@ -3195,14 +3195,14 @@
       <c r="E8" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="10" t="b">
-        <v>0</v>
+      <c r="F8" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="G8" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="H8" s="10" t="b">
-        <v>0</v>
+      <c r="H8" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="I8" s="10" t="b">
         <v>0</v>
@@ -3210,8 +3210,8 @@
       <c r="J8" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="K8" s="6" t="b">
-        <v>1</v>
+      <c r="K8" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="L8" s="10" t="b">
         <v>0</v>
@@ -3315,17 +3315,39 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="B9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="10" t="b">
+        <v>0</v>
+      </c>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>

</xml_diff>

<commit_message>
Finish All - Change
</commit_message>
<xml_diff>
--- a/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
+++ b/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="548">
   <si>
     <t>TITAN</t>
   </si>
@@ -1686,6 +1686,30 @@
   </si>
   <si>
     <t>464</t>
+  </si>
+  <si>
+    <t>INVALID</t>
+  </si>
+  <si>
+    <t>INVALID - GENERIC - Carry out 75,000km intermediate service</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -1887,7 +1911,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1966,10 +1990,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2266,7 +2287,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomRight" activeCell="AL16" sqref="AL16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2936,7 +2957,7 @@
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="6" t="b">
         <v>1</v>
       </c>
@@ -3058,20 +3079,18 @@
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>538</v>
-      </c>
-      <c r="B7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="10" t="b">
-        <v>0</v>
+      <c r="A7" s="27"/>
+      <c r="B7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="F7" s="6" t="b">
         <v>1</v>
@@ -3082,14 +3101,14 @@
       <c r="H7" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" s="10" t="b">
-        <v>0</v>
+      <c r="I7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="L7" s="10" t="b">
         <v>0</v>
@@ -3182,18 +3201,18 @@
       </c>
     </row>
     <row r="8" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10" t="b">
-        <v>0</v>
+      <c r="A8" s="28"/>
+      <c r="B8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="F8" s="6" t="b">
         <v>1</v>
@@ -3204,14 +3223,14 @@
       <c r="H8" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="I8" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="10" t="b">
-        <v>0</v>
+      <c r="I8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="L8" s="10" t="b">
         <v>0</v>
@@ -3314,7 +3333,9 @@
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="29" t="s">
+        <v>538</v>
+      </c>
       <c r="B9" s="6" t="b">
         <v>1</v>
       </c>
@@ -3327,20 +3348,20 @@
       <c r="E9" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="10" t="b">
-        <v>0</v>
+      <c r="F9" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="G9" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="H9" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="10" t="b">
-        <v>0</v>
+      <c r="H9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="K9" s="6" t="b">
         <v>1</v>
@@ -3348,37 +3369,99 @@
       <c r="L9" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="19"/>
-      <c r="X9" s="19"/>
-      <c r="Y9" s="19"/>
-      <c r="Z9" s="19"/>
-      <c r="AA9" s="19"/>
-      <c r="AB9" s="19"/>
-      <c r="AC9" s="19"/>
-      <c r="AD9" s="19"/>
-      <c r="AE9" s="19"/>
-      <c r="AF9" s="19"/>
-      <c r="AG9" s="19"/>
-      <c r="AH9" s="19"/>
-      <c r="AI9" s="19"/>
-      <c r="AJ9" s="19"/>
-      <c r="AK9" s="19"/>
-      <c r="AL9" s="19"/>
-      <c r="AM9" s="19"/>
-      <c r="AN9" s="19"/>
-      <c r="AO9" s="19"/>
-      <c r="AP9" s="19"/>
-      <c r="AQ9" s="19"/>
+      <c r="M9" s="10" t="s">
+        <v>535</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="19" t="s">
+        <v>529</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="T9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="U9" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="V9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="W9" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="X9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z9" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC9" s="20" t="s">
+        <v>536</v>
+      </c>
+      <c r="AD9" s="20" t="s">
+        <v>521</v>
+      </c>
+      <c r="AE9" s="20" t="s">
+        <v>537</v>
+      </c>
+      <c r="AF9" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG9" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH9" s="10" t="s">
+        <v>540</v>
+      </c>
+      <c r="AI9" s="21" t="s">
+        <v>541</v>
+      </c>
+      <c r="AJ9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL9" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="AM9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="AR9" s="22" t="s">
         <v>42</v>
       </c>
@@ -3422,10 +3505,18 @@
       <c r="AJ10" s="19"/>
       <c r="AK10" s="19"/>
       <c r="AL10" s="19"/>
-      <c r="AM10" s="19"/>
-      <c r="AN10" s="19"/>
-      <c r="AO10" s="19"/>
-      <c r="AP10" s="19"/>
+      <c r="AM10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN10" s="19" t="s">
+        <v>542</v>
+      </c>
+      <c r="AO10" s="19" t="s">
+        <v>542</v>
+      </c>
+      <c r="AP10" s="19" t="s">
+        <v>546</v>
+      </c>
       <c r="AQ10" s="19"/>
       <c r="AR10" s="22" t="s">
         <v>43</v>
@@ -3470,10 +3561,18 @@
       <c r="AJ11" s="19"/>
       <c r="AK11" s="19"/>
       <c r="AL11" s="19"/>
-      <c r="AM11" s="19"/>
-      <c r="AN11" s="19"/>
-      <c r="AO11" s="19"/>
-      <c r="AP11" s="19"/>
+      <c r="AM11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN11" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="AO11" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="AP11" s="19" t="s">
+        <v>547</v>
+      </c>
       <c r="AQ11" s="19"/>
       <c r="AR11" s="22" t="s">
         <v>44</v>
@@ -3518,9 +3617,15 @@
       <c r="AJ12" s="19"/>
       <c r="AK12" s="19"/>
       <c r="AL12" s="19"/>
-      <c r="AM12" s="19"/>
-      <c r="AN12" s="19"/>
-      <c r="AO12" s="19"/>
+      <c r="AM12" s="19" t="s">
+        <v>529</v>
+      </c>
+      <c r="AN12" s="19" t="s">
+        <v>544</v>
+      </c>
+      <c r="AO12" s="19" t="s">
+        <v>544</v>
+      </c>
       <c r="AP12" s="19"/>
       <c r="AQ12" s="19"/>
       <c r="AR12" s="22" t="s">
@@ -3567,8 +3672,12 @@
       <c r="AK13" s="19"/>
       <c r="AL13" s="19"/>
       <c r="AM13" s="19"/>
-      <c r="AN13" s="19"/>
-      <c r="AO13" s="19"/>
+      <c r="AN13" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="AO13" s="19" t="s">
+        <v>545</v>
+      </c>
       <c r="AP13" s="19"/>
       <c r="AQ13" s="19"/>
       <c r="AR13" s="22" t="s">
@@ -3912,7 +4021,9 @@
       </c>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="29" t="s">
+        <v>538</v>
+      </c>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -3960,7 +4071,7 @@
       </c>
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -25273,9 +25384,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:T1"/>
-  <mergeCells count="2">
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A8"/>
+  <mergeCells count="1">
+    <mergeCell ref="A3:A8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AA3" r:id="rId1"/>

</xml_diff>

<commit_message>
Done change Date, change Customer Vehicle 90%
</commit_message>
<xml_diff>
--- a/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
+++ b/Data Files/Holden/DATA_DRIVEN_HOLDEN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinh.le\git\TITAN_HOLDEN_API_BK\Data Files\Holden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinh.le\git\TITAN_HOLDEN_API\Data Files\Holden\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="548">
   <si>
     <t>TITAN</t>
   </si>
@@ -1980,6 +1980,9 @@
     <xf numFmtId="49" fontId="6" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1988,9 +1991,6 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2287,7 +2287,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="G9:H9"/>
+      <selection pane="bottomRight" activeCell="AM10" sqref="AM10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,7 +2589,7 @@
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>534</v>
       </c>
       <c r="B3" s="6" t="b">
@@ -2713,7 +2713,7 @@
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="6" t="b">
         <v>1</v>
       </c>
@@ -2835,7 +2835,7 @@
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="6" t="b">
         <v>1</v>
       </c>
@@ -2957,7 +2957,7 @@
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="6" t="b">
         <v>1</v>
       </c>
@@ -3079,7 +3079,7 @@
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="6" t="b">
         <v>1</v>
       </c>
@@ -3201,7 +3201,7 @@
       </c>
     </row>
     <row r="8" spans="1:44" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="6" t="b">
         <v>1</v>
       </c>
@@ -3333,7 +3333,7 @@
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="26" t="s">
         <v>538</v>
       </c>
       <c r="B9" s="6" t="b">
@@ -3447,8 +3447,8 @@
       <c r="AL9" s="11" t="s">
         <v>529</v>
       </c>
-      <c r="AM9" s="10" t="b">
-        <v>0</v>
+      <c r="AM9" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="AN9" s="10" t="b">
         <v>0</v>
@@ -4021,7 +4021,7 @@
       </c>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="26" t="s">
         <v>538</v>
       </c>
       <c r="B21" s="19"/>

</xml_diff>